<commit_message>
cleans up redd metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/clear_redd_metadata.xlsx
+++ b/data-raw/metadata/clear_redd_metadata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\jpe-deer-mill-adult-edi\data-raw\metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\jpe-clear-adult-edi\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB872A25-12E9-4A9C-90DF-1305F0320879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B6C5C2-962C-448E-BBE1-85DDB6D007F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40125" yWindow="870" windowWidth="25815" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26535" yWindow="1665" windowWidth="21600" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="64">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -118,12 +118,6 @@
     <t>YYYY</t>
   </si>
   <si>
-    <t>max_yearly_redd_count</t>
-  </si>
-  <si>
-    <t>Maximum number of fish counted</t>
-  </si>
-  <si>
     <t>1997-10-01</t>
   </si>
   <si>
@@ -142,10 +136,88 @@
     <t>redd</t>
   </si>
   <si>
-    <t>count of fish</t>
+    <t>integer</t>
   </si>
   <si>
-    <t>integer</t>
+    <t>river_mile</t>
+  </si>
+  <si>
+    <t>River mile associated with redd measured</t>
+  </si>
+  <si>
+    <t>redd_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unique redd ID </t>
+  </si>
+  <si>
+    <t>enumerated</t>
+  </si>
+  <si>
+    <t>fish_guarding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whether or not fish were observed guarding the redd (T/F) </t>
+  </si>
+  <si>
+    <t>redd_measured</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whether or not redd was measured (T/F)   </t>
+  </si>
+  <si>
+    <t>redd_width</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Width of redd measured (m)     </t>
+  </si>
+  <si>
+    <t>redd_length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Length of redd measured (m)  </t>
+  </si>
+  <si>
+    <t>velocity</t>
+  </si>
+  <si>
+    <t>Measured stream velocity (ft/s)</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age of redd   </t>
+  </si>
+  <si>
+    <t>Number of times redd was aged. If 0, redd was sampled but not aged</t>
+  </si>
+  <si>
+    <t>age_index</t>
+  </si>
+  <si>
+    <t>redd_count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of redds sampled    </t>
+  </si>
+  <si>
+    <t>run</t>
+  </si>
+  <si>
+    <t xml:space="preserve">survey_method </t>
+  </si>
+  <si>
+    <t>species</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Survey method </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run of fish associated with redd  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Species associated with redd </t>
   </si>
 </sst>
 </file>
@@ -215,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -249,6 +321,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,11 +537,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1003"/>
+  <dimension ref="A1:Z1016"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -542,55 +615,62 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>27</v>
+    <row r="2" spans="1:26" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>20</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>28</v>
+      <c r="B2" s="16" t="s">
+        <v>22</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>25</v>
+      <c r="C2" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>39</v>
-      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
       <c r="I2" s="6"/>
       <c r="J2" s="5" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="K2" s="6"/>
-      <c r="L2" s="5">
-        <v>1997</v>
+      <c r="L2" s="13" t="s">
+        <v>30</v>
       </c>
-      <c r="M2" s="5">
-        <v>2020</v>
+      <c r="M2" s="13" t="s">
+        <v>31</v>
       </c>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>26</v>
+      <c r="B3" s="16" t="s">
+        <v>34</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>13</v>
@@ -601,8 +681,8 @@
       <c r="I3" s="6"/>
       <c r="J3" s="5"/>
       <c r="K3" s="6"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
@@ -619,21 +699,23 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>37</v>
+      <c r="E4" s="4" t="s">
+        <v>15</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>13</v>
+      <c r="F4" s="5" t="s">
+        <v>14</v>
       </c>
-      <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="6"/>
@@ -657,38 +739,30 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>31</v>
+      <c r="B5" s="16" t="s">
+        <v>40</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>39</v>
-      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
       <c r="I5" s="6"/>
       <c r="J5" s="5"/>
       <c r="K5" s="6"/>
-      <c r="L5" s="5">
-        <v>0</v>
-      </c>
-      <c r="M5" s="5">
-        <v>172</v>
-      </c>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -705,34 +779,28 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="6"/>
-      <c r="J6" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="J6" s="5"/>
       <c r="K6" s="6"/>
-      <c r="L6" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="M6" s="13" t="s">
-        <v>33</v>
-      </c>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
@@ -748,19 +816,29 @@
       <c r="Z6" s="1"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="4"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="4"/>
+      <c r="A7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="I7" s="6"/>
       <c r="J7" s="5"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="5"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
@@ -776,19 +854,35 @@
       <c r="Z7" s="1"/>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="4"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="5"/>
+      <c r="A8" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
       <c r="I8" s="6"/>
       <c r="J8" s="5"/>
       <c r="K8" s="6"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
+      <c r="L8" s="19">
+        <v>0.43180089999999999</v>
+      </c>
+      <c r="M8" s="19">
+        <v>9.1440180000000009</v>
+      </c>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
@@ -804,19 +898,35 @@
       <c r="Z8" s="1"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="4"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="5"/>
+      <c r="A9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="6"/>
       <c r="J9" s="5"/>
       <c r="K9" s="6"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="12"/>
+      <c r="L9" s="19">
+        <v>0.63500129999999999</v>
+      </c>
+      <c r="M9" s="19">
+        <v>11.176019999999999</v>
+      </c>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -832,19 +942,35 @@
       <c r="Z9" s="1"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="4"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="5"/>
+      <c r="A10" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="6"/>
       <c r="J10" s="5"/>
       <c r="K10" s="6"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
+      <c r="L10" s="19">
+        <v>0.252</v>
+      </c>
+      <c r="M10" s="19">
+        <v>407.94810000000001</v>
+      </c>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
@@ -860,19 +986,35 @@
       <c r="Z10" s="1"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="5"/>
+      <c r="A11" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="6"/>
       <c r="J11" s="5"/>
       <c r="K11" s="6"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
+      <c r="L11" s="19">
+        <v>1</v>
+      </c>
+      <c r="M11" s="19">
+        <v>6</v>
+      </c>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
@@ -888,19 +1030,35 @@
       <c r="Z11" s="1"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="5"/>
+      <c r="A12" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="6"/>
       <c r="J12" s="5"/>
       <c r="K12" s="6"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
+      <c r="L12" s="19">
+        <v>0</v>
+      </c>
+      <c r="M12" s="19">
+        <v>9</v>
+      </c>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -916,19 +1074,35 @@
       <c r="Z12" s="1"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="5"/>
+      <c r="A13" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="6"/>
       <c r="J13" s="5"/>
       <c r="K13" s="6"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
+      <c r="L13" s="19">
+        <v>0</v>
+      </c>
+      <c r="M13" s="19">
+        <v>1</v>
+      </c>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
@@ -943,19 +1117,29 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="4"/>
+    <row r="14" spans="1:26" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="6"/>
       <c r="J14" s="5"/>
       <c r="K14" s="6"/>
-      <c r="L14" s="10"/>
+      <c r="L14" s="5"/>
       <c r="M14" s="5"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
@@ -972,102 +1156,115 @@
       <c r="Z14" s="1"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
+      <c r="A15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="I15" s="6"/>
-      <c r="J15" s="5"/>
+      <c r="J15" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="K15" s="6"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="1"/>
-      <c r="R15" s="1"/>
-      <c r="S15" s="1"/>
-      <c r="T15" s="1"/>
-      <c r="U15" s="1"/>
-      <c r="V15" s="1"/>
-      <c r="W15" s="1"/>
-      <c r="X15" s="1"/>
-      <c r="Y15" s="1"/>
-      <c r="Z15" s="1"/>
-    </row>
-    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="4"/>
+      <c r="L15" s="5">
+        <v>1997</v>
+      </c>
+      <c r="M15" s="5">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
       <c r="I16" s="6"/>
       <c r="J16" s="5"/>
       <c r="K16" s="6"/>
-      <c r="L16" s="10"/>
+      <c r="L16" s="5"/>
       <c r="M16" s="5"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
-      <c r="S16" s="1"/>
-      <c r="T16" s="1"/>
-      <c r="U16" s="1"/>
-      <c r="V16" s="1"/>
-      <c r="W16" s="1"/>
-      <c r="X16" s="1"/>
-      <c r="Y16" s="1"/>
-      <c r="Z16" s="1"/>
-    </row>
-    <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="4"/>
+    </row>
+    <row r="17" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
       <c r="I17" s="6"/>
       <c r="J17" s="5"/>
       <c r="K17" s="6"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
-      <c r="S17" s="1"/>
-      <c r="T17" s="1"/>
-      <c r="U17" s="1"/>
-      <c r="V17" s="1"/>
-      <c r="W17" s="1"/>
-      <c r="X17" s="1"/>
-      <c r="Y17" s="1"/>
-      <c r="Z17" s="1"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="4"/>
+      <c r="A18" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
       <c r="I18" s="6"/>
       <c r="J18" s="5"/>
       <c r="K18" s="6"/>
-      <c r="L18" s="12"/>
+      <c r="L18" s="5"/>
       <c r="M18" s="5"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
@@ -1083,37 +1280,9 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="12"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="1"/>
-      <c r="R19" s="1"/>
-      <c r="S19" s="1"/>
-      <c r="T19" s="1"/>
-      <c r="U19" s="1"/>
-      <c r="V19" s="1"/>
-      <c r="W19" s="1"/>
-      <c r="X19" s="1"/>
-      <c r="Y19" s="1"/>
-      <c r="Z19" s="1"/>
-    </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
+      <c r="B20" s="16"/>
       <c r="C20" s="4"/>
       <c r="D20" s="6"/>
       <c r="E20" s="4"/>
@@ -1122,8 +1291,8 @@
       <c r="H20" s="5"/>
       <c r="I20" s="6"/>
       <c r="J20" s="5"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="10"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="14"/>
       <c r="M20" s="5"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
@@ -1141,18 +1310,18 @@
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
@@ -1169,18 +1338,18 @@
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="12"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
@@ -1197,18 +1366,18 @@
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
@@ -1225,18 +1394,18 @@
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
@@ -1251,19 +1420,20 @@
       <c r="Y24" s="1"/>
       <c r="Z24" s="1"/>
     </row>
-    <row r="25" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="4"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
@@ -1280,18 +1450,18 @@
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="13"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
@@ -1308,18 +1478,18 @@
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="4"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="5"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
@@ -1336,18 +1506,18 @@
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="4"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="5"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
@@ -1364,18 +1534,18 @@
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="4"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="2"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="5"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
@@ -1392,18 +1562,18 @@
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="12"/>
+      <c r="M30" s="12"/>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
@@ -1420,18 +1590,18 @@
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="4"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="5"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
@@ -1448,58 +1618,59 @@
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="4"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="1"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="4"/>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
       <c r="I32" s="6"/>
       <c r="J32" s="5"/>
       <c r="K32" s="6"/>
-      <c r="L32" s="5"/>
+      <c r="L32" s="12"/>
       <c r="M32" s="5"/>
-      <c r="N32" s="4"/>
-      <c r="O32" s="4"/>
-      <c r="P32" s="4"/>
-      <c r="Q32" s="4"/>
-      <c r="R32" s="4"/>
-      <c r="S32" s="4"/>
-      <c r="T32" s="4"/>
-      <c r="U32" s="4"/>
-      <c r="V32" s="4"/>
-      <c r="W32" s="4"/>
-      <c r="X32" s="4"/>
-      <c r="Y32" s="4"/>
-      <c r="Z32" s="4"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="1"/>
+      <c r="U32" s="1"/>
+      <c r="V32" s="1"/>
+      <c r="W32" s="1"/>
+      <c r="X32" s="1"/>
+      <c r="Y32" s="1"/>
+      <c r="Z32" s="1"/>
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="4"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="1"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="4"/>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
       <c r="I33" s="6"/>
       <c r="J33" s="5"/>
       <c r="K33" s="6"/>
-      <c r="L33" s="5"/>
+      <c r="L33" s="10"/>
       <c r="M33" s="5"/>
-      <c r="N33" s="4"/>
-      <c r="O33" s="4"/>
-      <c r="P33" s="4"/>
-      <c r="Q33" s="4"/>
-      <c r="R33" s="4"/>
-      <c r="S33" s="4"/>
-      <c r="T33" s="4"/>
-      <c r="U33" s="4"/>
-      <c r="V33" s="4"/>
-      <c r="W33" s="4"/>
-      <c r="X33" s="4"/>
-      <c r="Y33" s="4"/>
-      <c r="Z33" s="4"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1"/>
+      <c r="S33" s="1"/>
+      <c r="T33" s="1"/>
+      <c r="U33" s="1"/>
+      <c r="V33" s="1"/>
+      <c r="W33" s="1"/>
+      <c r="X33" s="1"/>
+      <c r="Y33" s="1"/>
+      <c r="Z33" s="1"/>
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="4"/>
@@ -1530,6 +1701,16 @@
       <c r="Z34" s="1"/>
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="4"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="3"/>
       <c r="K35" s="2"/>
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
@@ -1603,9 +1784,8 @@
       <c r="Y37" s="1"/>
       <c r="Z37" s="1"/>
     </row>
-    <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="4"/>
-      <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="2"/>
       <c r="E38" s="1"/>
@@ -1688,6 +1868,7 @@
       <c r="Z40" s="1"/>
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="4"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="2"/>
@@ -1743,6 +1924,7 @@
       <c r="Z42" s="1"/>
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="4"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="2"/>
@@ -1799,31 +1981,30 @@
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="4"/>
-      <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="2"/>
       <c r="E45" s="1"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
-      <c r="H45" s="3"/>
-      <c r="I45" s="2"/>
-      <c r="J45" s="3"/>
-      <c r="K45" s="2"/>
-      <c r="L45" s="3"/>
-      <c r="M45" s="3"/>
-      <c r="N45" s="1"/>
-      <c r="O45" s="1"/>
-      <c r="P45" s="1"/>
-      <c r="Q45" s="1"/>
-      <c r="R45" s="1"/>
-      <c r="S45" s="1"/>
-      <c r="T45" s="1"/>
-      <c r="U45" s="1"/>
-      <c r="V45" s="1"/>
-      <c r="W45" s="1"/>
-      <c r="X45" s="1"/>
-      <c r="Y45" s="1"/>
-      <c r="Z45" s="1"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="6"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="6"/>
+      <c r="L45" s="5"/>
+      <c r="M45" s="5"/>
+      <c r="N45" s="4"/>
+      <c r="O45" s="4"/>
+      <c r="P45" s="4"/>
+      <c r="Q45" s="4"/>
+      <c r="R45" s="4"/>
+      <c r="S45" s="4"/>
+      <c r="T45" s="4"/>
+      <c r="U45" s="4"/>
+      <c r="V45" s="4"/>
+      <c r="W45" s="4"/>
+      <c r="X45" s="4"/>
+      <c r="Y45" s="4"/>
+      <c r="Z45" s="4"/>
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="4"/>
@@ -1831,27 +2012,27 @@
       <c r="C46" s="1"/>
       <c r="D46" s="2"/>
       <c r="E46" s="1"/>
-      <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
-      <c r="I46" s="2"/>
-      <c r="J46" s="3"/>
-      <c r="K46" s="2"/>
-      <c r="L46" s="3"/>
-      <c r="M46" s="3"/>
-      <c r="N46" s="1"/>
-      <c r="O46" s="1"/>
-      <c r="P46" s="1"/>
-      <c r="Q46" s="1"/>
-      <c r="R46" s="1"/>
-      <c r="S46" s="1"/>
-      <c r="T46" s="1"/>
-      <c r="U46" s="1"/>
-      <c r="V46" s="1"/>
-      <c r="W46" s="1"/>
-      <c r="X46" s="1"/>
-      <c r="Y46" s="1"/>
-      <c r="Z46" s="1"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="6"/>
+      <c r="J46" s="5"/>
+      <c r="K46" s="6"/>
+      <c r="L46" s="5"/>
+      <c r="M46" s="5"/>
+      <c r="N46" s="4"/>
+      <c r="O46" s="4"/>
+      <c r="P46" s="4"/>
+      <c r="Q46" s="4"/>
+      <c r="R46" s="4"/>
+      <c r="S46" s="4"/>
+      <c r="T46" s="4"/>
+      <c r="U46" s="4"/>
+      <c r="V46" s="4"/>
+      <c r="W46" s="4"/>
+      <c r="X46" s="4"/>
+      <c r="Y46" s="4"/>
+      <c r="Z46" s="4"/>
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="4"/>
@@ -1882,16 +2063,6 @@
       <c r="Z47" s="1"/>
     </row>
     <row r="48" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="4"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
-      <c r="I48" s="2"/>
-      <c r="J48" s="3"/>
       <c r="K48" s="2"/>
       <c r="L48" s="3"/>
       <c r="M48" s="3"/>
@@ -2050,7 +2221,6 @@
       <c r="Z53" s="1"/>
     </row>
     <row r="54" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="4"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="2"/>
@@ -2106,7 +2276,6 @@
       <c r="Z55" s="1"/>
     </row>
     <row r="56" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="4"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="2"/>
@@ -2722,7 +2891,7 @@
       <c r="Z77" s="1"/>
     </row>
     <row r="78" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="1"/>
+      <c r="A78" s="4"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
       <c r="D78" s="2"/>
@@ -2750,7 +2919,7 @@
       <c r="Z78" s="1"/>
     </row>
     <row r="79" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="1"/>
+      <c r="A79" s="4"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="2"/>
@@ -2778,7 +2947,7 @@
       <c r="Z79" s="1"/>
     </row>
     <row r="80" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="1"/>
+      <c r="A80" s="4"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="2"/>
@@ -2806,7 +2975,7 @@
       <c r="Z80" s="1"/>
     </row>
     <row r="81" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="1"/>
+      <c r="A81" s="4"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="2"/>
@@ -2834,7 +3003,7 @@
       <c r="Z81" s="1"/>
     </row>
     <row r="82" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="1"/>
+      <c r="A82" s="4"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="2"/>
@@ -2862,7 +3031,7 @@
       <c r="Z82" s="1"/>
     </row>
     <row r="83" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="1"/>
+      <c r="A83" s="4"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="2"/>
@@ -2890,7 +3059,7 @@
       <c r="Z83" s="1"/>
     </row>
     <row r="84" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="1"/>
+      <c r="A84" s="4"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
       <c r="D84" s="2"/>
@@ -2918,7 +3087,7 @@
       <c r="Z84" s="1"/>
     </row>
     <row r="85" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="1"/>
+      <c r="A85" s="4"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
       <c r="D85" s="2"/>
@@ -2946,7 +3115,7 @@
       <c r="Z85" s="1"/>
     </row>
     <row r="86" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="1"/>
+      <c r="A86" s="4"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
       <c r="D86" s="2"/>
@@ -2974,7 +3143,7 @@
       <c r="Z86" s="1"/>
     </row>
     <row r="87" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="1"/>
+      <c r="A87" s="4"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
       <c r="D87" s="2"/>
@@ -3002,7 +3171,7 @@
       <c r="Z87" s="1"/>
     </row>
     <row r="88" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="1"/>
+      <c r="A88" s="4"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
       <c r="D88" s="2"/>
@@ -3030,7 +3199,7 @@
       <c r="Z88" s="1"/>
     </row>
     <row r="89" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A89" s="1"/>
+      <c r="A89" s="4"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
       <c r="D89" s="2"/>
@@ -3058,7 +3227,7 @@
       <c r="Z89" s="1"/>
     </row>
     <row r="90" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A90" s="1"/>
+      <c r="A90" s="4"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
       <c r="D90" s="2"/>
@@ -28649,18 +28818,382 @@
       <c r="Y1003" s="1"/>
       <c r="Z1003" s="1"/>
     </row>
+    <row r="1004" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1004" s="1"/>
+      <c r="B1004" s="1"/>
+      <c r="C1004" s="1"/>
+      <c r="D1004" s="2"/>
+      <c r="E1004" s="1"/>
+      <c r="F1004" s="3"/>
+      <c r="G1004" s="3"/>
+      <c r="H1004" s="3"/>
+      <c r="I1004" s="2"/>
+      <c r="J1004" s="3"/>
+      <c r="K1004" s="2"/>
+      <c r="L1004" s="3"/>
+      <c r="M1004" s="3"/>
+      <c r="N1004" s="1"/>
+      <c r="O1004" s="1"/>
+      <c r="P1004" s="1"/>
+      <c r="Q1004" s="1"/>
+      <c r="R1004" s="1"/>
+      <c r="S1004" s="1"/>
+      <c r="T1004" s="1"/>
+      <c r="U1004" s="1"/>
+      <c r="V1004" s="1"/>
+      <c r="W1004" s="1"/>
+      <c r="X1004" s="1"/>
+      <c r="Y1004" s="1"/>
+      <c r="Z1004" s="1"/>
+    </row>
+    <row r="1005" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1005" s="1"/>
+      <c r="B1005" s="1"/>
+      <c r="C1005" s="1"/>
+      <c r="D1005" s="2"/>
+      <c r="E1005" s="1"/>
+      <c r="F1005" s="3"/>
+      <c r="G1005" s="3"/>
+      <c r="H1005" s="3"/>
+      <c r="I1005" s="2"/>
+      <c r="J1005" s="3"/>
+      <c r="K1005" s="2"/>
+      <c r="L1005" s="3"/>
+      <c r="M1005" s="3"/>
+      <c r="N1005" s="1"/>
+      <c r="O1005" s="1"/>
+      <c r="P1005" s="1"/>
+      <c r="Q1005" s="1"/>
+      <c r="R1005" s="1"/>
+      <c r="S1005" s="1"/>
+      <c r="T1005" s="1"/>
+      <c r="U1005" s="1"/>
+      <c r="V1005" s="1"/>
+      <c r="W1005" s="1"/>
+      <c r="X1005" s="1"/>
+      <c r="Y1005" s="1"/>
+      <c r="Z1005" s="1"/>
+    </row>
+    <row r="1006" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1006" s="1"/>
+      <c r="B1006" s="1"/>
+      <c r="C1006" s="1"/>
+      <c r="D1006" s="2"/>
+      <c r="E1006" s="1"/>
+      <c r="F1006" s="3"/>
+      <c r="G1006" s="3"/>
+      <c r="H1006" s="3"/>
+      <c r="I1006" s="2"/>
+      <c r="J1006" s="3"/>
+      <c r="K1006" s="2"/>
+      <c r="L1006" s="3"/>
+      <c r="M1006" s="3"/>
+      <c r="N1006" s="1"/>
+      <c r="O1006" s="1"/>
+      <c r="P1006" s="1"/>
+      <c r="Q1006" s="1"/>
+      <c r="R1006" s="1"/>
+      <c r="S1006" s="1"/>
+      <c r="T1006" s="1"/>
+      <c r="U1006" s="1"/>
+      <c r="V1006" s="1"/>
+      <c r="W1006" s="1"/>
+      <c r="X1006" s="1"/>
+      <c r="Y1006" s="1"/>
+      <c r="Z1006" s="1"/>
+    </row>
+    <row r="1007" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1007" s="1"/>
+      <c r="B1007" s="1"/>
+      <c r="C1007" s="1"/>
+      <c r="D1007" s="2"/>
+      <c r="E1007" s="1"/>
+      <c r="F1007" s="3"/>
+      <c r="G1007" s="3"/>
+      <c r="H1007" s="3"/>
+      <c r="I1007" s="2"/>
+      <c r="J1007" s="3"/>
+      <c r="K1007" s="2"/>
+      <c r="L1007" s="3"/>
+      <c r="M1007" s="3"/>
+      <c r="N1007" s="1"/>
+      <c r="O1007" s="1"/>
+      <c r="P1007" s="1"/>
+      <c r="Q1007" s="1"/>
+      <c r="R1007" s="1"/>
+      <c r="S1007" s="1"/>
+      <c r="T1007" s="1"/>
+      <c r="U1007" s="1"/>
+      <c r="V1007" s="1"/>
+      <c r="W1007" s="1"/>
+      <c r="X1007" s="1"/>
+      <c r="Y1007" s="1"/>
+      <c r="Z1007" s="1"/>
+    </row>
+    <row r="1008" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1008" s="1"/>
+      <c r="B1008" s="1"/>
+      <c r="C1008" s="1"/>
+      <c r="D1008" s="2"/>
+      <c r="E1008" s="1"/>
+      <c r="F1008" s="3"/>
+      <c r="G1008" s="3"/>
+      <c r="H1008" s="3"/>
+      <c r="I1008" s="2"/>
+      <c r="J1008" s="3"/>
+      <c r="K1008" s="2"/>
+      <c r="L1008" s="3"/>
+      <c r="M1008" s="3"/>
+      <c r="N1008" s="1"/>
+      <c r="O1008" s="1"/>
+      <c r="P1008" s="1"/>
+      <c r="Q1008" s="1"/>
+      <c r="R1008" s="1"/>
+      <c r="S1008" s="1"/>
+      <c r="T1008" s="1"/>
+      <c r="U1008" s="1"/>
+      <c r="V1008" s="1"/>
+      <c r="W1008" s="1"/>
+      <c r="X1008" s="1"/>
+      <c r="Y1008" s="1"/>
+      <c r="Z1008" s="1"/>
+    </row>
+    <row r="1009" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1009" s="1"/>
+      <c r="B1009" s="1"/>
+      <c r="C1009" s="1"/>
+      <c r="D1009" s="2"/>
+      <c r="E1009" s="1"/>
+      <c r="F1009" s="3"/>
+      <c r="G1009" s="3"/>
+      <c r="H1009" s="3"/>
+      <c r="I1009" s="2"/>
+      <c r="J1009" s="3"/>
+      <c r="K1009" s="2"/>
+      <c r="L1009" s="3"/>
+      <c r="M1009" s="3"/>
+      <c r="N1009" s="1"/>
+      <c r="O1009" s="1"/>
+      <c r="P1009" s="1"/>
+      <c r="Q1009" s="1"/>
+      <c r="R1009" s="1"/>
+      <c r="S1009" s="1"/>
+      <c r="T1009" s="1"/>
+      <c r="U1009" s="1"/>
+      <c r="V1009" s="1"/>
+      <c r="W1009" s="1"/>
+      <c r="X1009" s="1"/>
+      <c r="Y1009" s="1"/>
+      <c r="Z1009" s="1"/>
+    </row>
+    <row r="1010" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1010" s="1"/>
+      <c r="B1010" s="1"/>
+      <c r="C1010" s="1"/>
+      <c r="D1010" s="2"/>
+      <c r="E1010" s="1"/>
+      <c r="F1010" s="3"/>
+      <c r="G1010" s="3"/>
+      <c r="H1010" s="3"/>
+      <c r="I1010" s="2"/>
+      <c r="J1010" s="3"/>
+      <c r="K1010" s="2"/>
+      <c r="L1010" s="3"/>
+      <c r="M1010" s="3"/>
+      <c r="N1010" s="1"/>
+      <c r="O1010" s="1"/>
+      <c r="P1010" s="1"/>
+      <c r="Q1010" s="1"/>
+      <c r="R1010" s="1"/>
+      <c r="S1010" s="1"/>
+      <c r="T1010" s="1"/>
+      <c r="U1010" s="1"/>
+      <c r="V1010" s="1"/>
+      <c r="W1010" s="1"/>
+      <c r="X1010" s="1"/>
+      <c r="Y1010" s="1"/>
+      <c r="Z1010" s="1"/>
+    </row>
+    <row r="1011" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1011" s="1"/>
+      <c r="B1011" s="1"/>
+      <c r="C1011" s="1"/>
+      <c r="D1011" s="2"/>
+      <c r="E1011" s="1"/>
+      <c r="F1011" s="3"/>
+      <c r="G1011" s="3"/>
+      <c r="H1011" s="3"/>
+      <c r="I1011" s="2"/>
+      <c r="J1011" s="3"/>
+      <c r="K1011" s="2"/>
+      <c r="L1011" s="3"/>
+      <c r="M1011" s="3"/>
+      <c r="N1011" s="1"/>
+      <c r="O1011" s="1"/>
+      <c r="P1011" s="1"/>
+      <c r="Q1011" s="1"/>
+      <c r="R1011" s="1"/>
+      <c r="S1011" s="1"/>
+      <c r="T1011" s="1"/>
+      <c r="U1011" s="1"/>
+      <c r="V1011" s="1"/>
+      <c r="W1011" s="1"/>
+      <c r="X1011" s="1"/>
+      <c r="Y1011" s="1"/>
+      <c r="Z1011" s="1"/>
+    </row>
+    <row r="1012" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1012" s="1"/>
+      <c r="B1012" s="1"/>
+      <c r="C1012" s="1"/>
+      <c r="D1012" s="2"/>
+      <c r="E1012" s="1"/>
+      <c r="F1012" s="3"/>
+      <c r="G1012" s="3"/>
+      <c r="H1012" s="3"/>
+      <c r="I1012" s="2"/>
+      <c r="J1012" s="3"/>
+      <c r="K1012" s="2"/>
+      <c r="L1012" s="3"/>
+      <c r="M1012" s="3"/>
+      <c r="N1012" s="1"/>
+      <c r="O1012" s="1"/>
+      <c r="P1012" s="1"/>
+      <c r="Q1012" s="1"/>
+      <c r="R1012" s="1"/>
+      <c r="S1012" s="1"/>
+      <c r="T1012" s="1"/>
+      <c r="U1012" s="1"/>
+      <c r="V1012" s="1"/>
+      <c r="W1012" s="1"/>
+      <c r="X1012" s="1"/>
+      <c r="Y1012" s="1"/>
+      <c r="Z1012" s="1"/>
+    </row>
+    <row r="1013" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1013" s="1"/>
+      <c r="B1013" s="1"/>
+      <c r="C1013" s="1"/>
+      <c r="D1013" s="2"/>
+      <c r="E1013" s="1"/>
+      <c r="F1013" s="3"/>
+      <c r="G1013" s="3"/>
+      <c r="H1013" s="3"/>
+      <c r="I1013" s="2"/>
+      <c r="J1013" s="3"/>
+      <c r="K1013" s="2"/>
+      <c r="L1013" s="3"/>
+      <c r="M1013" s="3"/>
+      <c r="N1013" s="1"/>
+      <c r="O1013" s="1"/>
+      <c r="P1013" s="1"/>
+      <c r="Q1013" s="1"/>
+      <c r="R1013" s="1"/>
+      <c r="S1013" s="1"/>
+      <c r="T1013" s="1"/>
+      <c r="U1013" s="1"/>
+      <c r="V1013" s="1"/>
+      <c r="W1013" s="1"/>
+      <c r="X1013" s="1"/>
+      <c r="Y1013" s="1"/>
+      <c r="Z1013" s="1"/>
+    </row>
+    <row r="1014" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1014" s="1"/>
+      <c r="B1014" s="1"/>
+      <c r="C1014" s="1"/>
+      <c r="D1014" s="2"/>
+      <c r="E1014" s="1"/>
+      <c r="F1014" s="3"/>
+      <c r="G1014" s="3"/>
+      <c r="H1014" s="3"/>
+      <c r="I1014" s="2"/>
+      <c r="J1014" s="3"/>
+      <c r="K1014" s="2"/>
+      <c r="L1014" s="3"/>
+      <c r="M1014" s="3"/>
+      <c r="N1014" s="1"/>
+      <c r="O1014" s="1"/>
+      <c r="P1014" s="1"/>
+      <c r="Q1014" s="1"/>
+      <c r="R1014" s="1"/>
+      <c r="S1014" s="1"/>
+      <c r="T1014" s="1"/>
+      <c r="U1014" s="1"/>
+      <c r="V1014" s="1"/>
+      <c r="W1014" s="1"/>
+      <c r="X1014" s="1"/>
+      <c r="Y1014" s="1"/>
+      <c r="Z1014" s="1"/>
+    </row>
+    <row r="1015" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1015" s="1"/>
+      <c r="B1015" s="1"/>
+      <c r="C1015" s="1"/>
+      <c r="D1015" s="2"/>
+      <c r="E1015" s="1"/>
+      <c r="F1015" s="3"/>
+      <c r="G1015" s="3"/>
+      <c r="H1015" s="3"/>
+      <c r="I1015" s="2"/>
+      <c r="J1015" s="3"/>
+      <c r="K1015" s="2"/>
+      <c r="L1015" s="3"/>
+      <c r="M1015" s="3"/>
+      <c r="N1015" s="1"/>
+      <c r="O1015" s="1"/>
+      <c r="P1015" s="1"/>
+      <c r="Q1015" s="1"/>
+      <c r="R1015" s="1"/>
+      <c r="S1015" s="1"/>
+      <c r="T1015" s="1"/>
+      <c r="U1015" s="1"/>
+      <c r="V1015" s="1"/>
+      <c r="W1015" s="1"/>
+      <c r="X1015" s="1"/>
+      <c r="Y1015" s="1"/>
+      <c r="Z1015" s="1"/>
+    </row>
+    <row r="1016" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1016" s="1"/>
+      <c r="B1016" s="1"/>
+      <c r="C1016" s="1"/>
+      <c r="D1016" s="2"/>
+      <c r="E1016" s="1"/>
+      <c r="F1016" s="3"/>
+      <c r="G1016" s="3"/>
+      <c r="H1016" s="3"/>
+      <c r="I1016" s="2"/>
+      <c r="J1016" s="3"/>
+      <c r="K1016" s="2"/>
+      <c r="L1016" s="3"/>
+      <c r="M1016" s="3"/>
+      <c r="N1016" s="1"/>
+      <c r="O1016" s="1"/>
+      <c r="P1016" s="1"/>
+      <c r="Q1016" s="1"/>
+      <c r="R1016" s="1"/>
+      <c r="S1016" s="1"/>
+      <c r="T1016" s="1"/>
+      <c r="U1016" s="1"/>
+      <c r="V1016" s="1"/>
+      <c r="W1016" s="1"/>
+      <c r="X1016" s="1"/>
+      <c r="Y1016" s="1"/>
+      <c r="Z1016" s="1"/>
+    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C60:C1003 C36:C48 C1:C34" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C73:C1016 C49:C61 C20:C47 C1:C18" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E36:E1003 E1:E34" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E49:E1016 E20:E47 E1:E18" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F36:F1003 F1:F34" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F49:F1016 F20:F47 F1:F18" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"ratio,interval"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H36:H1003 H1:H34" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H49:H1016 H20:H47 H1:H18" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
xml validates, metadata checked
</commit_message>
<xml_diff>
--- a/data-raw/metadata/clear_redd_metadata.xlsx
+++ b/data-raw/metadata/clear_redd_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\jpe-clear-adult-edi\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E762DC-84E6-40FF-B57E-B1945C6745C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C55A1CF-08D7-4378-998C-685FAE88BEF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16665" yWindow="855" windowWidth="14235" windowHeight="14670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="860" yWindow="2070" windowWidth="20880" windowHeight="13130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="69">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -145,9 +145,6 @@
     <t xml:space="preserve">Unique redd ID </t>
   </si>
   <si>
-    <t>enumerated</t>
-  </si>
-  <si>
     <t>fish_guarding</t>
   </si>
   <si>
@@ -227,6 +224,15 @@
   </si>
   <si>
     <t>whole</t>
+  </si>
+  <si>
+    <t>meter</t>
+  </si>
+  <si>
+    <t>feetPerSecond</t>
+  </si>
+  <si>
+    <t>count of redd</t>
   </si>
 </sst>
 </file>
@@ -549,7 +555,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -648,10 +654,10 @@
       </c>
       <c r="K2" s="6"/>
       <c r="L2" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M2" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -719,15 +725,11 @@
         <v>33</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>14</v>
-      </c>
+      <c r="F4" s="5"/>
       <c r="G4" s="5"/>
-      <c r="H4" s="5" t="s">
-        <v>64</v>
-      </c>
+      <c r="H4" s="5"/>
       <c r="I4" s="6"/>
       <c r="J4" s="5"/>
       <c r="K4" s="6"/>
@@ -761,11 +763,9 @@
         <v>33</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>25</v>
-      </c>
+      <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="6"/>
@@ -789,10 +789,10 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>23</v>
@@ -827,10 +827,10 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>23</v>
@@ -865,10 +865,10 @@
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>14</v>
@@ -882,9 +882,11 @@
       <c r="F8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="5"/>
+      <c r="G8" s="5" t="s">
+        <v>66</v>
+      </c>
       <c r="H8" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I8" s="6"/>
       <c r="J8" s="5"/>
@@ -911,10 +913,10 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>14</v>
@@ -928,9 +930,11 @@
       <c r="F9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="5"/>
+      <c r="G9" s="5" t="s">
+        <v>66</v>
+      </c>
       <c r="H9" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I9" s="6"/>
       <c r="J9" s="5"/>
@@ -957,10 +961,10 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>14</v>
@@ -974,9 +978,11 @@
       <c r="F10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="5"/>
+      <c r="G10" s="5" t="s">
+        <v>67</v>
+      </c>
       <c r="H10" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="5"/>
@@ -1003,10 +1009,10 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>14</v>
@@ -1020,9 +1026,11 @@
       <c r="F11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="5"/>
+      <c r="G11" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="H11" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="5"/>
@@ -1049,10 +1057,10 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>31</v>
@@ -1061,15 +1069,11 @@
         <v>33</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>25</v>
-      </c>
+      <c r="F12" s="5"/>
       <c r="G12" s="5"/>
-      <c r="H12" s="5" t="s">
-        <v>66</v>
-      </c>
+      <c r="H12" s="5"/>
       <c r="I12" s="6"/>
       <c r="J12" s="5"/>
       <c r="K12" s="6"/>
@@ -1095,10 +1099,10 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>14</v>
@@ -1112,9 +1116,11 @@
       <c r="F13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="5"/>
+      <c r="G13" s="5" t="s">
+        <v>68</v>
+      </c>
       <c r="H13" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="5"/>
@@ -1216,10 +1222,10 @@
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>23</v>
@@ -1241,10 +1247,10 @@
     </row>
     <row r="17" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>23</v>
@@ -1266,10 +1272,10 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
renames files from escapement to upstream passage. removes redunant stream column from tables and updates metadata. adds levels of categorical variables to metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/clear_redd_metadata.xlsx
+++ b/data-raw/metadata/clear_redd_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-clear-adult-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC3F56FD-516E-EB42-92A2-FF64D84C6348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B80A146-A746-E341-B683-250122D46E57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="61">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -100,19 +100,7 @@
     <t>nominal</t>
   </si>
   <si>
-    <t>stream</t>
-  </si>
-  <si>
-    <t>Name of the stream where data is collected</t>
-  </si>
-  <si>
     <t>year</t>
-  </si>
-  <si>
-    <t>Year the upstream passage data were recorded</t>
-  </si>
-  <si>
-    <t>YYYY</t>
   </si>
   <si>
     <t>reach</t>
@@ -121,16 +109,10 @@
     <t>ordinal</t>
   </si>
   <si>
-    <t>Survey reach</t>
-  </si>
-  <si>
     <t>redd</t>
   </si>
   <si>
     <t>river_mile</t>
-  </si>
-  <si>
-    <t>River mile associated with redd measured</t>
   </si>
   <si>
     <t>redd_id</t>
@@ -154,19 +136,10 @@
     <t>redd_width</t>
   </si>
   <si>
-    <t xml:space="preserve">Width of redd measured (m)     </t>
-  </si>
-  <si>
     <t>redd_length</t>
   </si>
   <si>
-    <t xml:space="preserve">Length of redd measured (m)  </t>
-  </si>
-  <si>
     <t>velocity</t>
-  </si>
-  <si>
-    <t>Measured stream velocity (ft/s)</t>
   </si>
   <si>
     <t>age</t>
@@ -193,12 +166,6 @@
     <t xml:space="preserve">survey_method </t>
   </si>
   <si>
-    <t xml:space="preserve">Survey method </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Run of fish associated with redd  </t>
-  </si>
-  <si>
     <t>2000-09-25</t>
   </si>
   <si>
@@ -221,6 +188,27 @@
   </si>
   <si>
     <t>count of redds</t>
+  </si>
+  <si>
+    <t>Survey reach. Levels = c("R1", "R2", "R4", "R5", "R3", "R6A", "R7")</t>
+  </si>
+  <si>
+    <t>River mile where the redd was measured</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Width of redd measured  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Length of redd measured </t>
+  </si>
+  <si>
+    <t>Measured stream velocity</t>
+  </si>
+  <si>
+    <t>Survey method. Levels = c("snorkel", "rstr", "pw")</t>
+  </si>
+  <si>
+    <t>Run of fish associated with redd. Levels = c("spring")</t>
   </si>
 </sst>
 </file>
@@ -539,11 +527,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1015"/>
+  <dimension ref="A1:Z1013"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -628,7 +616,7 @@
         <v>16</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>16</v>
@@ -642,10 +630,10 @@
       </c>
       <c r="K2" s="6"/>
       <c r="L2" s="13" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="M2" s="13" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -663,16 +651,16 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>13</v>
@@ -701,16 +689,16 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>13</v>
@@ -739,16 +727,16 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>13</v>
@@ -777,16 +765,16 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>13</v>
@@ -815,16 +803,16 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>13</v>
@@ -853,16 +841,16 @@
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>15</v>
@@ -871,10 +859,10 @@
         <v>14</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="I8" s="6"/>
       <c r="J8" s="5"/>
@@ -901,16 +889,16 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>15</v>
@@ -919,10 +907,10 @@
         <v>14</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="I9" s="6"/>
       <c r="J9" s="5"/>
@@ -949,16 +937,16 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>15</v>
@@ -967,10 +955,10 @@
         <v>14</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="5"/>
@@ -997,16 +985,16 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>15</v>
@@ -1015,10 +1003,10 @@
         <v>14</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="5"/>
@@ -1045,16 +1033,16 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>13</v>
@@ -1087,16 +1075,16 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>15</v>
@@ -1105,10 +1093,10 @@
         <v>14</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="5"/>
@@ -1133,18 +1121,18 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14" spans="1:26" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>25</v>
+      <c r="B14" s="9" t="s">
+        <v>59</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>13</v>
@@ -1157,100 +1145,87 @@
       <c r="K14" s="6"/>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
-      <c r="S14" s="1"/>
-      <c r="T14" s="1"/>
-      <c r="U14" s="1"/>
-      <c r="V14" s="1"/>
-      <c r="W14" s="1"/>
-      <c r="X14" s="1"/>
-      <c r="Y14" s="1"/>
-      <c r="Z14" s="1"/>
-    </row>
-    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>26</v>
+    </row>
+    <row r="15" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>44</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>32</v>
-      </c>
       <c r="E15" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
       <c r="I15" s="6"/>
-      <c r="J15" s="5" t="s">
-        <v>28</v>
-      </c>
+      <c r="J15" s="5"/>
       <c r="K15" s="6"/>
-      <c r="L15" s="5">
-        <v>1997</v>
-      </c>
-      <c r="M15" s="5">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-    </row>
-    <row r="17" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+    </row>
+    <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="4"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
       <c r="I17" s="6"/>
       <c r="J17" s="5"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="5"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="14"/>
       <c r="M17" s="5"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
+    </row>
+    <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="4"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1"/>
+      <c r="Y18" s="1"/>
+      <c r="Z18" s="1"/>
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
@@ -1263,9 +1238,9 @@
       <c r="H19" s="5"/>
       <c r="I19" s="6"/>
       <c r="J19" s="5"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="5"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="18"/>
+      <c r="M19" s="12"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
@@ -1282,7 +1257,7 @@
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
-      <c r="B20" s="16"/>
+      <c r="B20" s="17"/>
       <c r="C20" s="4"/>
       <c r="D20" s="6"/>
       <c r="E20" s="4"/>
@@ -1292,8 +1267,8 @@
       <c r="I20" s="6"/>
       <c r="J20" s="5"/>
       <c r="K20" s="6"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
@@ -1310,7 +1285,7 @@
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
-      <c r="B21" s="16"/>
+      <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="6"/>
       <c r="E21" s="4"/>
@@ -1320,8 +1295,8 @@
       <c r="I21" s="6"/>
       <c r="J21" s="5"/>
       <c r="K21" s="6"/>
-      <c r="L21" s="18"/>
-      <c r="M21" s="12"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
@@ -1338,7 +1313,7 @@
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
-      <c r="B22" s="17"/>
+      <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="6"/>
       <c r="E22" s="4"/>
@@ -1348,8 +1323,8 @@
       <c r="I22" s="6"/>
       <c r="J22" s="5"/>
       <c r="K22" s="6"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
@@ -1376,8 +1351,8 @@
       <c r="I23" s="6"/>
       <c r="J23" s="5"/>
       <c r="K23" s="6"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
@@ -1404,7 +1379,7 @@
       <c r="I24" s="6"/>
       <c r="J24" s="5"/>
       <c r="K24" s="6"/>
-      <c r="L24" s="5"/>
+      <c r="L24" s="10"/>
       <c r="M24" s="5"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
@@ -1432,8 +1407,8 @@
       <c r="I25" s="6"/>
       <c r="J25" s="5"/>
       <c r="K25" s="6"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="5"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
@@ -1488,8 +1463,8 @@
       <c r="I27" s="6"/>
       <c r="J27" s="5"/>
       <c r="K27" s="6"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="5"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
@@ -1516,7 +1491,7 @@
       <c r="I28" s="6"/>
       <c r="J28" s="5"/>
       <c r="K28" s="6"/>
-      <c r="L28" s="10"/>
+      <c r="L28" s="12"/>
       <c r="M28" s="5"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
@@ -1545,7 +1520,7 @@
       <c r="J29" s="5"/>
       <c r="K29" s="6"/>
       <c r="L29" s="12"/>
-      <c r="M29" s="12"/>
+      <c r="M29" s="5"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
@@ -1572,7 +1547,7 @@
       <c r="I30" s="6"/>
       <c r="J30" s="5"/>
       <c r="K30" s="6"/>
-      <c r="L30" s="12"/>
+      <c r="L30" s="10"/>
       <c r="M30" s="5"/>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
@@ -1590,18 +1565,18 @@
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="12"/>
-      <c r="M31" s="5"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
@@ -1618,18 +1593,18 @@
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="5"/>
-      <c r="K32" s="6"/>
-      <c r="L32" s="10"/>
-      <c r="M32" s="5"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
@@ -1700,9 +1675,8 @@
       <c r="Y34" s="1"/>
       <c r="Z34" s="1"/>
     </row>
-    <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4"/>
-      <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="2"/>
       <c r="E35" s="1"/>
@@ -1756,8 +1730,9 @@
       <c r="Y36" s="1"/>
       <c r="Z36" s="1"/>
     </row>
-    <row r="37" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4"/>
+      <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="2"/>
       <c r="E37" s="1"/>
@@ -1897,31 +1872,30 @@
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4"/>
-      <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="2"/>
       <c r="E42" s="1"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="3"/>
-      <c r="K42" s="2"/>
-      <c r="L42" s="3"/>
-      <c r="M42" s="3"/>
-      <c r="N42" s="1"/>
-      <c r="O42" s="1"/>
-      <c r="P42" s="1"/>
-      <c r="Q42" s="1"/>
-      <c r="R42" s="1"/>
-      <c r="S42" s="1"/>
-      <c r="T42" s="1"/>
-      <c r="U42" s="1"/>
-      <c r="V42" s="1"/>
-      <c r="W42" s="1"/>
-      <c r="X42" s="1"/>
-      <c r="Y42" s="1"/>
-      <c r="Z42" s="1"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="5"/>
+      <c r="K42" s="6"/>
+      <c r="L42" s="5"/>
+      <c r="M42" s="5"/>
+      <c r="N42" s="4"/>
+      <c r="O42" s="4"/>
+      <c r="P42" s="4"/>
+      <c r="Q42" s="4"/>
+      <c r="R42" s="4"/>
+      <c r="S42" s="4"/>
+      <c r="T42" s="4"/>
+      <c r="U42" s="4"/>
+      <c r="V42" s="4"/>
+      <c r="W42" s="4"/>
+      <c r="X42" s="4"/>
+      <c r="Y42" s="4"/>
+      <c r="Z42" s="4"/>
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4"/>
@@ -1929,82 +1903,73 @@
       <c r="C43" s="1"/>
       <c r="D43" s="2"/>
       <c r="E43" s="1"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="2"/>
-      <c r="J43" s="3"/>
-      <c r="K43" s="2"/>
-      <c r="L43" s="3"/>
-      <c r="M43" s="3"/>
-      <c r="N43" s="1"/>
-      <c r="O43" s="1"/>
-      <c r="P43" s="1"/>
-      <c r="Q43" s="1"/>
-      <c r="R43" s="1"/>
-      <c r="S43" s="1"/>
-      <c r="T43" s="1"/>
-      <c r="U43" s="1"/>
-      <c r="V43" s="1"/>
-      <c r="W43" s="1"/>
-      <c r="X43" s="1"/>
-      <c r="Y43" s="1"/>
-      <c r="Z43" s="1"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="6"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="6"/>
+      <c r="L43" s="5"/>
+      <c r="M43" s="5"/>
+      <c r="N43" s="4"/>
+      <c r="O43" s="4"/>
+      <c r="P43" s="4"/>
+      <c r="Q43" s="4"/>
+      <c r="R43" s="4"/>
+      <c r="S43" s="4"/>
+      <c r="T43" s="4"/>
+      <c r="U43" s="4"/>
+      <c r="V43" s="4"/>
+      <c r="W43" s="4"/>
+      <c r="X43" s="4"/>
+      <c r="Y43" s="4"/>
+      <c r="Z43" s="4"/>
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4"/>
+      <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="2"/>
       <c r="E44" s="1"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
-      <c r="H44" s="5"/>
-      <c r="I44" s="6"/>
-      <c r="J44" s="5"/>
-      <c r="K44" s="6"/>
-      <c r="L44" s="5"/>
-      <c r="M44" s="5"/>
-      <c r="N44" s="4"/>
-      <c r="O44" s="4"/>
-      <c r="P44" s="4"/>
-      <c r="Q44" s="4"/>
-      <c r="R44" s="4"/>
-      <c r="S44" s="4"/>
-      <c r="T44" s="4"/>
-      <c r="U44" s="4"/>
-      <c r="V44" s="4"/>
-      <c r="W44" s="4"/>
-      <c r="X44" s="4"/>
-      <c r="Y44" s="4"/>
-      <c r="Z44" s="4"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="3"/>
+      <c r="M44" s="3"/>
+      <c r="N44" s="1"/>
+      <c r="O44" s="1"/>
+      <c r="P44" s="1"/>
+      <c r="Q44" s="1"/>
+      <c r="R44" s="1"/>
+      <c r="S44" s="1"/>
+      <c r="T44" s="1"/>
+      <c r="U44" s="1"/>
+      <c r="V44" s="1"/>
+      <c r="W44" s="1"/>
+      <c r="X44" s="1"/>
+      <c r="Y44" s="1"/>
+      <c r="Z44" s="1"/>
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="4"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="5"/>
-      <c r="G45" s="5"/>
-      <c r="H45" s="5"/>
-      <c r="I45" s="6"/>
-      <c r="J45" s="5"/>
-      <c r="K45" s="6"/>
-      <c r="L45" s="5"/>
-      <c r="M45" s="5"/>
-      <c r="N45" s="4"/>
-      <c r="O45" s="4"/>
-      <c r="P45" s="4"/>
-      <c r="Q45" s="4"/>
-      <c r="R45" s="4"/>
-      <c r="S45" s="4"/>
-      <c r="T45" s="4"/>
-      <c r="U45" s="4"/>
-      <c r="V45" s="4"/>
-      <c r="W45" s="4"/>
-      <c r="X45" s="4"/>
-      <c r="Y45" s="4"/>
-      <c r="Z45" s="4"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="3"/>
+      <c r="M45" s="3"/>
+      <c r="N45" s="1"/>
+      <c r="O45" s="1"/>
+      <c r="P45" s="1"/>
+      <c r="Q45" s="1"/>
+      <c r="R45" s="1"/>
+      <c r="S45" s="1"/>
+      <c r="T45" s="1"/>
+      <c r="U45" s="1"/>
+      <c r="V45" s="1"/>
+      <c r="W45" s="1"/>
+      <c r="X45" s="1"/>
+      <c r="Y45" s="1"/>
+      <c r="Z45" s="1"/>
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="4"/>
@@ -2035,6 +2000,16 @@
       <c r="Z46" s="1"/>
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="4"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="3"/>
       <c r="K47" s="2"/>
       <c r="L47" s="3"/>
       <c r="M47" s="3"/>
@@ -2137,7 +2112,6 @@
       <c r="Z50" s="1"/>
     </row>
     <row r="51" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="4"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="2"/>
@@ -2248,6 +2222,7 @@
       <c r="Z54" s="1"/>
     </row>
     <row r="55" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="4"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="2"/>
@@ -3171,7 +3146,7 @@
       <c r="Z87" s="1"/>
     </row>
     <row r="88" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="4"/>
+      <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
       <c r="D88" s="2"/>
@@ -3199,7 +3174,7 @@
       <c r="Z88" s="1"/>
     </row>
     <row r="89" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="4"/>
+      <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
       <c r="D89" s="2"/>
@@ -29098,74 +29073,18 @@
       <c r="Y1013" s="1"/>
       <c r="Z1013" s="1"/>
     </row>
-    <row r="1014" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1014" s="1"/>
-      <c r="B1014" s="1"/>
-      <c r="C1014" s="1"/>
-      <c r="D1014" s="2"/>
-      <c r="E1014" s="1"/>
-      <c r="F1014" s="3"/>
-      <c r="G1014" s="3"/>
-      <c r="H1014" s="3"/>
-      <c r="I1014" s="2"/>
-      <c r="J1014" s="3"/>
-      <c r="K1014" s="2"/>
-      <c r="L1014" s="3"/>
-      <c r="M1014" s="3"/>
-      <c r="N1014" s="1"/>
-      <c r="O1014" s="1"/>
-      <c r="P1014" s="1"/>
-      <c r="Q1014" s="1"/>
-      <c r="R1014" s="1"/>
-      <c r="S1014" s="1"/>
-      <c r="T1014" s="1"/>
-      <c r="U1014" s="1"/>
-      <c r="V1014" s="1"/>
-      <c r="W1014" s="1"/>
-      <c r="X1014" s="1"/>
-      <c r="Y1014" s="1"/>
-      <c r="Z1014" s="1"/>
-    </row>
-    <row r="1015" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1015" s="1"/>
-      <c r="B1015" s="1"/>
-      <c r="C1015" s="1"/>
-      <c r="D1015" s="2"/>
-      <c r="E1015" s="1"/>
-      <c r="F1015" s="3"/>
-      <c r="G1015" s="3"/>
-      <c r="H1015" s="3"/>
-      <c r="I1015" s="2"/>
-      <c r="J1015" s="3"/>
-      <c r="K1015" s="2"/>
-      <c r="L1015" s="3"/>
-      <c r="M1015" s="3"/>
-      <c r="N1015" s="1"/>
-      <c r="O1015" s="1"/>
-      <c r="P1015" s="1"/>
-      <c r="Q1015" s="1"/>
-      <c r="R1015" s="1"/>
-      <c r="S1015" s="1"/>
-      <c r="T1015" s="1"/>
-      <c r="U1015" s="1"/>
-      <c r="V1015" s="1"/>
-      <c r="W1015" s="1"/>
-      <c r="X1015" s="1"/>
-      <c r="Y1015" s="1"/>
-      <c r="Z1015" s="1"/>
-    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C72:C1015 C48:C60 C19:C46 C1:C17" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C70:C1013 C46:C58 C17:C44 C1:C15" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E48:E1015 E19:E46 E1:E17" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E46:E1013 E17:E44 E1:E15" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F48:F1015 F19:F46 F1:F17" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F46:F1013 F17:F44 F1:F15" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"ratio,interval"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H48:H1015 H19:H46 H1:H17" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H46:H1013 H17:H44 H1:H15" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
fixes typo in redd metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/clear_redd_metadata.xlsx
+++ b/data-raw/metadata/clear_redd_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/SRJPE/EDI/jpe-clear-adult-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C5C664F-E354-574D-8102-AAB020D84BF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37CD7C52-BCFD-884B-9EA0-4E5DA798F5BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-200" yWindow="760" windowWidth="19520" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="19520" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -232,7 +232,7 @@
 "fine gravel", "coarse gravel to boulder")</t>
   </si>
   <si>
-    <t>Run of the fish on the redd. Run is determined fprimarily by whether or not the redd was observed above or below a picket weir installed near a natural barrier. Years prior to 2003 do not have the picket weir information, but are considered reliable for run assignment. Levels = c("spring")</t>
+    <t>Run of the fish on the redd. Run is determined primarily by whether or not the redd was observed above or below a picket weir installed near a natural barrier. Years prior to 2003 do not have the picket weir information, but are considered reliable for run assignment. Levels = c("spring")</t>
   </si>
 </sst>
 </file>
@@ -557,7 +557,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
adds redd summary table
</commit_message>
<xml_diff>
--- a/data-raw/metadata/clear_redd_metadata.xlsx
+++ b/data-raw/metadata/clear_redd_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/SRJPE/EDI/jpe-clear-adult-edi/data-raw/metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleyvizek/code/jpe-clear-adult-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37CD7C52-BCFD-884B-9EA0-4E5DA798F5BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D81B607-FFD8-3A40-B0E0-CC7362DD1A4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="19520" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19520" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -154,9 +154,6 @@
     <t>feetPerSecond</t>
   </si>
   <si>
-    <t>count of redds</t>
-  </si>
-  <si>
     <t>Measured stream velocity</t>
   </si>
   <si>
@@ -233,6 +230,9 @@
   </si>
   <si>
     <t>Run of the fish on the redd. Run is determined primarily by whether or not the redd was observed above or below a picket weir installed near a natural barrier. Years prior to 2003 do not have the picket weir information, but are considered reliable for run assignment. Levels = c("spring")</t>
+  </si>
+  <si>
+    <t>number of redds</t>
   </si>
 </sst>
 </file>
@@ -557,7 +557,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -637,7 +637,7 @@
         <v>20</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>16</v>
@@ -681,7 +681,7 @@
         <v>27</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>22</v>
@@ -719,7 +719,7 @@
         <v>24</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>25</v>
@@ -754,10 +754,10 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>22</v>
@@ -843,7 +843,7 @@
         <v>35</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>22</v>
@@ -868,7 +868,7 @@
         <v>34</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>14</v>
@@ -883,10 +883,10 @@
         <v>14</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="6"/>
@@ -916,7 +916,7 @@
         <v>28</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>22</v>
@@ -954,7 +954,7 @@
         <v>29</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>14</v>
@@ -1002,7 +1002,7 @@
         <v>30</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>14</v>
@@ -1047,10 +1047,10 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>14</v>
@@ -1065,7 +1065,7 @@
         <v>14</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H12" s="6" t="s">
         <v>38</v>
@@ -1095,10 +1095,10 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>14</v>
@@ -1113,7 +1113,7 @@
         <v>14</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H13" s="6" t="s">
         <v>38</v>
@@ -1143,10 +1143,10 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>14</v>
@@ -1161,7 +1161,7 @@
         <v>14</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H14" s="6" t="s">
         <v>38</v>
@@ -1191,10 +1191,10 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>22</v>
@@ -1229,10 +1229,10 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>22</v>
@@ -1267,10 +1267,10 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>22</v>
@@ -1308,7 +1308,7 @@
         <v>31</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
adds 2020 and 2022-2023 redd data
</commit_message>
<xml_diff>
--- a/data-raw/metadata/clear_redd_metadata.xlsx
+++ b/data-raw/metadata/clear_redd_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleyvizek/code/jpe-clear-adult-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D81B607-FFD8-3A40-B0E0-CC7362DD1A4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BBCD92D-C9A1-DA41-9386-D16C982BC2B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19520" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19520" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="64">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -130,9 +130,6 @@
     <t xml:space="preserve">Age of redd   </t>
   </si>
   <si>
-    <t>redd_count</t>
-  </si>
-  <si>
     <t>run</t>
   </si>
   <si>
@@ -157,9 +154,6 @@
     <t>Measured stream velocity</t>
   </si>
   <si>
-    <t>integer</t>
-  </si>
-  <si>
     <t>Date of redd survey</t>
   </si>
   <si>
@@ -173,9 +167,6 @@
   </si>
   <si>
     <t>Whether or not a fish was observed on the redd being sampled. Levels = c("NA", "TRUE", "FALSE")</t>
-  </si>
-  <si>
-    <t>Number of redds counted.</t>
   </si>
   <si>
     <t>Whether or not the redd was measured at time of observation. Levels = c(FALSE, TRUE)</t>
@@ -230,9 +221,6 @@
   </si>
   <si>
     <t>Run of the fish on the redd. Run is determined primarily by whether or not the redd was observed above or below a picket weir installed near a natural barrier. Years prior to 2003 do not have the picket weir information, but are considered reliable for run assignment. Levels = c("spring")</t>
-  </si>
-  <si>
-    <t>number of redds</t>
   </si>
 </sst>
 </file>
@@ -553,11 +541,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1016"/>
+  <dimension ref="A1:Z1015"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -637,7 +625,7 @@
         <v>20</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>16</v>
@@ -657,10 +645,10 @@
       </c>
       <c r="K2" s="5"/>
       <c r="L2" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N2" s="7"/>
       <c r="O2" s="7"/>
@@ -681,7 +669,7 @@
         <v>27</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>22</v>
@@ -719,7 +707,7 @@
         <v>24</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>25</v>
@@ -754,10 +742,10 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>22</v>
@@ -813,7 +801,7 @@
         <v>23</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I6" s="5"/>
       <c r="J6" s="6"/>
@@ -840,10 +828,10 @@
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>22</v>
@@ -865,38 +853,28 @@
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>49</v>
+      <c r="B8" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>26</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>43</v>
-      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
       <c r="I8" s="5"/>
       <c r="J8" s="6"/>
       <c r="K8" s="5"/>
-      <c r="L8" s="6">
-        <v>0</v>
-      </c>
-      <c r="M8" s="6">
-        <v>1</v>
-      </c>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
       <c r="P8" s="7"/>
@@ -913,28 +891,38 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>26</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
+      <c r="F9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="I9" s="5"/>
       <c r="J9" s="6"/>
       <c r="K9" s="5"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
+      <c r="L9" s="6">
+        <v>0.43180089999999999</v>
+      </c>
+      <c r="M9" s="6">
+        <v>9.1440180000000009</v>
+      </c>
       <c r="N9" s="7"/>
       <c r="O9" s="7"/>
       <c r="P9" s="7"/>
@@ -951,10 +939,10 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>14</v>
@@ -969,19 +957,19 @@
         <v>14</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I10" s="5"/>
       <c r="J10" s="6"/>
       <c r="K10" s="5"/>
       <c r="L10" s="6">
-        <v>0.43180089999999999</v>
+        <v>0.63500129999999999</v>
       </c>
       <c r="M10" s="6">
-        <v>9.1440180000000009</v>
+        <v>11.176019999999999</v>
       </c>
       <c r="N10" s="7"/>
       <c r="O10" s="7"/>
@@ -999,10 +987,10 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>14</v>
@@ -1017,19 +1005,19 @@
         <v>14</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="6"/>
       <c r="K11" s="5"/>
       <c r="L11" s="6">
-        <v>0.63500129999999999</v>
+        <v>0.12700030000000001</v>
       </c>
       <c r="M11" s="6">
-        <v>11.176019999999999</v>
+        <v>2.2352045</v>
       </c>
       <c r="N11" s="7"/>
       <c r="O11" s="7"/>
@@ -1047,10 +1035,10 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>14</v>
@@ -1065,19 +1053,19 @@
         <v>14</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I12" s="5"/>
       <c r="J12" s="6"/>
       <c r="K12" s="5"/>
       <c r="L12" s="6">
-        <v>0.12700030000000001</v>
+        <v>0.15240029999999999</v>
       </c>
       <c r="M12" s="6">
-        <v>2.2352045</v>
+        <v>2.4130047999999999</v>
       </c>
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
@@ -1095,10 +1083,10 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>14</v>
@@ -1113,19 +1101,19 @@
         <v>14</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="6"/>
       <c r="K13" s="5"/>
       <c r="L13" s="6">
-        <v>0.15240029999999999</v>
+        <v>7.6200149999999994E-2</v>
       </c>
       <c r="M13" s="6">
-        <v>2.4130047999999999</v>
+        <v>2.1336042700000002</v>
       </c>
       <c r="N13" s="7"/>
       <c r="O13" s="7"/>
@@ -1143,38 +1131,28 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>58</v>
+      <c r="B14" s="7" t="s">
+        <v>60</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>26</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
-      <c r="F14" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>38</v>
-      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
       <c r="I14" s="5"/>
       <c r="J14" s="6"/>
       <c r="K14" s="5"/>
-      <c r="L14" s="6">
-        <v>7.6200149999999994E-2</v>
-      </c>
-      <c r="M14" s="6">
-        <v>2.1336042700000002</v>
-      </c>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
       <c r="N14" s="7"/>
       <c r="O14" s="7"/>
       <c r="P14" s="7"/>
@@ -1191,10 +1169,10 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>22</v>
@@ -1229,10 +1207,10 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>22</v>
@@ -1267,28 +1245,38 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>65</v>
+      <c r="B17" s="8" t="s">
+        <v>41</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>26</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
+      <c r="F17" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="I17" s="5"/>
       <c r="J17" s="6"/>
       <c r="K17" s="5"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
+      <c r="L17" s="6">
+        <v>0.252</v>
+      </c>
+      <c r="M17" s="6">
+        <v>407.94810000000001</v>
+      </c>
       <c r="N17" s="7"/>
       <c r="O17" s="7"/>
       <c r="P17" s="7"/>
@@ -1303,53 +1291,30 @@
       <c r="Y17" s="7"/>
       <c r="Z17" s="7"/>
     </row>
-    <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="I18" s="5"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="6">
-        <v>0.252</v>
-      </c>
-      <c r="M18" s="6">
-        <v>407.94810000000001</v>
-      </c>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7"/>
-      <c r="Q18" s="7"/>
-      <c r="R18" s="7"/>
-      <c r="S18" s="7"/>
-      <c r="T18" s="7"/>
-      <c r="U18" s="7"/>
-      <c r="V18" s="7"/>
-      <c r="W18" s="7"/>
-      <c r="X18" s="7"/>
-      <c r="Y18" s="7"/>
-      <c r="Z18" s="7"/>
+    <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="8"/>
+      <c r="D19" s="5"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
+      <c r="U19" s="7"/>
+      <c r="V19" s="7"/>
+      <c r="W19" s="7"/>
+      <c r="X19" s="7"/>
+      <c r="Y19" s="7"/>
+      <c r="Z19" s="7"/>
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="8"/>
@@ -1359,9 +1324,9 @@
       <c r="H20" s="6"/>
       <c r="I20" s="5"/>
       <c r="J20" s="6"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="11"/>
-      <c r="M20" s="6"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
       <c r="N20" s="7"/>
       <c r="O20" s="7"/>
       <c r="P20" s="7"/>
@@ -1385,8 +1350,8 @@
       <c r="I21" s="5"/>
       <c r="J21" s="6"/>
       <c r="K21" s="5"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="13"/>
       <c r="N21" s="7"/>
       <c r="O21" s="7"/>
       <c r="P21" s="7"/>
@@ -1410,8 +1375,8 @@
       <c r="I22" s="5"/>
       <c r="J22" s="6"/>
       <c r="K22" s="5"/>
-      <c r="L22" s="12"/>
-      <c r="M22" s="13"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
       <c r="N22" s="7"/>
       <c r="O22" s="7"/>
       <c r="P22" s="7"/>
@@ -1427,7 +1392,6 @@
       <c r="Z22" s="7"/>
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="8"/>
       <c r="D23" s="5"/>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
@@ -1435,8 +1399,8 @@
       <c r="I23" s="5"/>
       <c r="J23" s="6"/>
       <c r="K23" s="5"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="14"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
       <c r="N23" s="7"/>
       <c r="O23" s="7"/>
       <c r="P23" s="7"/>
@@ -1483,8 +1447,8 @@
       <c r="I25" s="5"/>
       <c r="J25" s="6"/>
       <c r="K25" s="5"/>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
       <c r="N25" s="7"/>
       <c r="O25" s="7"/>
       <c r="P25" s="7"/>
@@ -1507,8 +1471,8 @@
       <c r="I26" s="5"/>
       <c r="J26" s="6"/>
       <c r="K26" s="5"/>
-      <c r="L26" s="9"/>
-      <c r="M26" s="9"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="6"/>
       <c r="N26" s="7"/>
       <c r="O26" s="7"/>
       <c r="P26" s="7"/>
@@ -1579,8 +1543,8 @@
       <c r="I29" s="5"/>
       <c r="J29" s="6"/>
       <c r="K29" s="5"/>
-      <c r="L29" s="15"/>
-      <c r="M29" s="6"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="13"/>
       <c r="N29" s="7"/>
       <c r="O29" s="7"/>
       <c r="P29" s="7"/>
@@ -1604,7 +1568,7 @@
       <c r="J30" s="6"/>
       <c r="K30" s="5"/>
       <c r="L30" s="13"/>
-      <c r="M30" s="13"/>
+      <c r="M30" s="6"/>
       <c r="N30" s="7"/>
       <c r="O30" s="7"/>
       <c r="P30" s="7"/>
@@ -1651,7 +1615,7 @@
       <c r="I32" s="5"/>
       <c r="J32" s="6"/>
       <c r="K32" s="5"/>
-      <c r="L32" s="13"/>
+      <c r="L32" s="15"/>
       <c r="M32" s="6"/>
       <c r="N32" s="7"/>
       <c r="O32" s="7"/>
@@ -1668,15 +1632,18 @@
       <c r="Z32" s="7"/>
     </row>
     <row r="33" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D33" s="5"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="5"/>
-      <c r="J33" s="6"/>
-      <c r="K33" s="5"/>
-      <c r="L33" s="15"/>
-      <c r="M33" s="6"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="17"/>
+      <c r="K33" s="16"/>
+      <c r="L33" s="17"/>
+      <c r="M33" s="17"/>
       <c r="N33" s="7"/>
       <c r="O33" s="7"/>
       <c r="P33" s="7"/>
@@ -1772,8 +1739,7 @@
       <c r="Y36" s="7"/>
       <c r="Z36" s="7"/>
     </row>
-    <row r="37" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="7"/>
+    <row r="37" spans="2:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C37" s="7"/>
       <c r="D37" s="16"/>
       <c r="E37" s="7"/>
@@ -1799,7 +1765,8 @@
       <c r="Y37" s="7"/>
       <c r="Z37" s="7"/>
     </row>
-    <row r="38" spans="2:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="7"/>
       <c r="C38" s="7"/>
       <c r="D38" s="16"/>
       <c r="E38" s="7"/>
@@ -1961,33 +1928,20 @@
       <c r="Z43" s="7"/>
     </row>
     <row r="44" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="7"/>
       <c r="C44" s="7"/>
       <c r="D44" s="16"/>
       <c r="E44" s="7"/>
-      <c r="F44" s="17"/>
-      <c r="G44" s="17"/>
-      <c r="H44" s="17"/>
-      <c r="I44" s="16"/>
-      <c r="J44" s="17"/>
-      <c r="K44" s="16"/>
-      <c r="L44" s="17"/>
-      <c r="M44" s="17"/>
-      <c r="N44" s="7"/>
-      <c r="O44" s="7"/>
-      <c r="P44" s="7"/>
-      <c r="Q44" s="7"/>
-      <c r="R44" s="7"/>
-      <c r="S44" s="7"/>
-      <c r="T44" s="7"/>
-      <c r="U44" s="7"/>
-      <c r="V44" s="7"/>
-      <c r="W44" s="7"/>
-      <c r="X44" s="7"/>
-      <c r="Y44" s="7"/>
-      <c r="Z44" s="7"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
+      <c r="I44" s="5"/>
+      <c r="J44" s="6"/>
+      <c r="K44" s="5"/>
+      <c r="L44" s="6"/>
+      <c r="M44" s="6"/>
     </row>
     <row r="45" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="7"/>
       <c r="C45" s="7"/>
       <c r="D45" s="16"/>
       <c r="E45" s="7"/>
@@ -2005,25 +1959,29 @@
       <c r="C46" s="7"/>
       <c r="D46" s="16"/>
       <c r="E46" s="7"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
-      <c r="H46" s="6"/>
-      <c r="I46" s="5"/>
-      <c r="J46" s="6"/>
-      <c r="K46" s="5"/>
-      <c r="L46" s="6"/>
-      <c r="M46" s="6"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="17"/>
+      <c r="H46" s="17"/>
+      <c r="I46" s="16"/>
+      <c r="J46" s="17"/>
+      <c r="K46" s="16"/>
+      <c r="L46" s="17"/>
+      <c r="M46" s="17"/>
+      <c r="N46" s="7"/>
+      <c r="O46" s="7"/>
+      <c r="P46" s="7"/>
+      <c r="Q46" s="7"/>
+      <c r="R46" s="7"/>
+      <c r="S46" s="7"/>
+      <c r="T46" s="7"/>
+      <c r="U46" s="7"/>
+      <c r="V46" s="7"/>
+      <c r="W46" s="7"/>
+      <c r="X46" s="7"/>
+      <c r="Y46" s="7"/>
+      <c r="Z46" s="7"/>
     </row>
     <row r="47" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="17"/>
-      <c r="G47" s="17"/>
-      <c r="H47" s="17"/>
-      <c r="I47" s="16"/>
-      <c r="J47" s="17"/>
       <c r="K47" s="16"/>
       <c r="L47" s="17"/>
       <c r="M47" s="17"/>
@@ -2042,6 +2000,15 @@
       <c r="Z47" s="7"/>
     </row>
     <row r="48" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B48" s="7"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="17"/>
+      <c r="G48" s="17"/>
+      <c r="H48" s="17"/>
+      <c r="I48" s="16"/>
+      <c r="J48" s="17"/>
       <c r="K48" s="16"/>
       <c r="L48" s="17"/>
       <c r="M48" s="17"/>
@@ -3167,6 +3134,7 @@
       <c r="Z89" s="7"/>
     </row>
     <row r="90" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="7"/>
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
       <c r="D90" s="16"/>
@@ -29093,46 +29061,18 @@
       <c r="Y1015" s="7"/>
       <c r="Z1015" s="7"/>
     </row>
-    <row r="1016" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1016" s="7"/>
-      <c r="B1016" s="7"/>
-      <c r="C1016" s="7"/>
-      <c r="D1016" s="16"/>
-      <c r="E1016" s="7"/>
-      <c r="F1016" s="17"/>
-      <c r="G1016" s="17"/>
-      <c r="H1016" s="17"/>
-      <c r="I1016" s="16"/>
-      <c r="J1016" s="17"/>
-      <c r="K1016" s="16"/>
-      <c r="L1016" s="17"/>
-      <c r="M1016" s="17"/>
-      <c r="N1016" s="7"/>
-      <c r="O1016" s="7"/>
-      <c r="P1016" s="7"/>
-      <c r="Q1016" s="7"/>
-      <c r="R1016" s="7"/>
-      <c r="S1016" s="7"/>
-      <c r="T1016" s="7"/>
-      <c r="U1016" s="7"/>
-      <c r="V1016" s="7"/>
-      <c r="W1016" s="7"/>
-      <c r="X1016" s="7"/>
-      <c r="Y1016" s="7"/>
-      <c r="Z1016" s="7"/>
-    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C73:C1016 C49:C61 C20:C47 C1:C18" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C72:C1015 C48:C60 C19:C46 C1:C17" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E49:E1016 E20:E47 E1:E18" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E48:E1015 E19:E46 E1:E17" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F49:F1016 F20:F47 F1:F18" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F48:F1015 F19:F46 F1:F17" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"ratio,interval"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H49:H1016 H20:H47 H1:H18" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H48:H1015 H19:H46 H1:H17" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>